<commit_message>
Yo weaklt monthly yearly :wink:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5AD5F1-F6E1-4FA1-8DDE-4F38BC9C9077}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF3BB08-EC84-45EB-B4F0-578985D669C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -217,6 +217,27 @@
   </si>
   <si>
     <t>SQL</t>
+  </si>
+  <si>
+    <t>frmRecloserFunction.vb</t>
+  </si>
+  <si>
+    <t>آذربایجان غربی ـ ایجاد امکان ثبت کارکرد ریکلوزر در نرم افزار (فرم جدید) ـ</t>
+  </si>
+  <si>
+    <t>آذربایجان غربی ـ ایجاد امکان ثبت کارکرد ریکلوزر ـ بخش دوم</t>
+  </si>
+  <si>
+    <t>frmBaseTablesNotStd.vb</t>
+  </si>
+  <si>
+    <t>آذربایجان غربی ـ ایجاد یک گزارش و با فیلترهای درخواستی در نامه برای ثبت کارکرد ریکلوزرها</t>
+  </si>
+  <si>
+    <t>Report_Recloser_Function.mrt</t>
+  </si>
+  <si>
+    <t>frmReportRecloser.vb</t>
   </si>
 </sst>
 </file>
@@ -471,83 +492,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -562,7 +506,86 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:K2"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +879,8 @@
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="5" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="35.140625" customWidth="1"/>
-    <col min="9" max="10" width="26.7109375" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" customWidth="1"/>
     <col min="11" max="11" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -890,36 +914,38 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="E2" s="27" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="E2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29"/>
-      <c r="I2" s="41" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="I2" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="43"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="E3" s="35" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="E3" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="I3" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -927,69 +953,98 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="I4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="E5" s="26" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="E5" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="E7" s="12" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="E7" s="20" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="13" t="s">
         <v>40</v>
       </c>
+      <c r="I7" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="I8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
@@ -997,18 +1052,23 @@
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="8" t="s">
@@ -1020,26 +1080,31 @@
       <c r="G10" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="I10" s="44"/>
+      <c r="J10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="E12" s="12" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="E12" s="20" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="10" t="s">
@@ -1048,48 +1113,48 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="6" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="E15" s="11" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="E15" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="E16" s="22" t="s">
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="E16" s="40" t="s">
         <v>49</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1100,40 +1165,40 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="37" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="23"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="43" t="s">
         <v>56</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1142,68 +1207,68 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="24" t="s">
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="42" t="s">
         <v>54</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="33" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="24"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="42"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="34"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="43" t="s">
         <v>35</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="12" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1211,7 +1276,7 @@
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="25"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="6" t="s">
         <v>39</v>
       </c>
@@ -1223,8 +1288,8 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="38"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>61</v>
       </c>
@@ -1233,35 +1298,41 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
+      <c r="E27" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
+      <c r="E28" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
+  <mergeCells count="38">
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:I10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="A20:C20"/>
@@ -1277,6 +1348,23 @@
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E24:E26"/>
     <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Report 'Report Sabz_Erja  (Old form of 14_4)' :weary:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF3BB08-EC84-45EB-B4F0-578985D669C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4953C2B-37E1-4528-AA58-90595ED337D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="76">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -238,6 +238,21 @@
   </si>
   <si>
     <t>frmReportRecloser.vb</t>
+  </si>
+  <si>
+    <t>Report Sabz_Erja  (Old form of 14_4)</t>
+  </si>
+  <si>
+    <t>spGetReport_Sabz_Erja</t>
+  </si>
+  <si>
+    <t>frmMainErja.vb</t>
+  </si>
+  <si>
+    <t>frmReportGreen</t>
+  </si>
+  <si>
+    <t>غرب مازندران ـ ايجاد گزارشات آماري درخواستي برای خدمات غیر حضوری سبز ـ بخش اول</t>
   </si>
 </sst>
 </file>
@@ -497,6 +512,77 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -506,31 +592,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,52 +600,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,7 +884,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,38 +929,38 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="E2" s="23" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="E2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
-      <c r="I2" s="14" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
+      <c r="I2" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="E3" s="26" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="E3" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
-      <c r="I3" s="29" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="I3" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -953,12 +968,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
-      <c r="I4" s="20" t="s">
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="I4" s="15" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -967,17 +982,17 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="E5" s="29" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="E5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="I5" s="44"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="1" t="s">
         <v>67</v>
       </c>
@@ -991,24 +1006,24 @@
       <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="I6" s="44"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="E7" s="20" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="E7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1017,11 +1032,11 @@
       <c r="G7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -1031,14 +1046,14 @@
       <c r="C8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="15" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -1047,24 +1062,24 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="E9" s="22" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="E9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="I9" s="44"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="1" t="s">
         <v>70</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1080,81 +1095,105 @@
       <c r="G10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="44"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="I11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="E12" s="20" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="E12" s="15" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G12" s="1"/>
+      <c r="I12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="21"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="6" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="7"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="E15" s="22" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="E15" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="E16" s="40" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="E16" s="27" t="s">
         <v>49</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1165,7 +1204,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1174,31 +1213,31 @@
       <c r="C17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="41"/>
+      <c r="E17" s="28"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="30" t="s">
         <v>56</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1207,19 +1246,19 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="42" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="29" t="s">
         <v>54</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1228,41 +1267,41 @@
       <c r="C21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="42"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="19"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="30" t="s">
         <v>35</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1276,7 +1315,7 @@
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="43"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="6" t="s">
         <v>39</v>
       </c>
@@ -1288,7 +1327,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="43"/>
+      <c r="E26" s="30"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>61</v>
@@ -1298,15 +1337,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="15" t="s">
         <v>23</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1316,7 +1355,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="21"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1326,15 +1365,24 @@
       <c r="A30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:E13"/>
+  <mergeCells count="41">
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A16:C16"/>
@@ -1344,27 +1392,21 @@
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="E19:E21"/>
     <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E14:G14"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E24:E26"/>
     <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Get Data updated ...
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4953C2B-37E1-4528-AA58-90595ED337D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA80C6E-5B02-41AA-81D3-1AFEBBBF2C90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -42,9 +42,6 @@
     <t>ایلام ـ ایجاد فیلتر «شماره دستور کار» در بخش گزارشات تکی اقلام مصرفی سرویس</t>
   </si>
   <si>
-    <t>Task</t>
-  </si>
-  <si>
     <t>Froms and Stuffs</t>
   </si>
   <si>
@@ -253,6 +250,36 @@
   </si>
   <si>
     <t>غرب مازندران ـ ايجاد گزارشات آماري درخواستي برای خدمات غیر حضوری سبز ـ بخش اول</t>
+  </si>
+  <si>
+    <t>آذربایجان غربی ـ تهیه وب سرویس با شرح خدمات درج شده</t>
+  </si>
+  <si>
+    <t>Report_AzarGH_FeederPeak</t>
+  </si>
+  <si>
+    <t>Report_AzarGH_PostFeederLoad</t>
+  </si>
+  <si>
+    <t>spGetReport_FeederPeak</t>
+  </si>
+  <si>
+    <t>spGetReport_PostFeederLoad</t>
+  </si>
+  <si>
+    <t>8th Week (1400/2/07)</t>
+  </si>
+  <si>
+    <t>7th Week (1400/3/1)</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>&lt;Host-Name&gt;/Reports/azargh_postfeederload</t>
+  </si>
+  <si>
+    <t>&lt;Host-Name&gt;/Reports/azargh_feederpeak</t>
   </si>
 </sst>
 </file>
@@ -512,94 +539,94 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -881,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,492 +924,559 @@
     <col min="9" max="9" width="26.7109375" customWidth="1"/>
     <col min="10" max="10" width="29.28515625" customWidth="1"/>
     <col min="11" max="11" width="35.7109375" customWidth="1"/>
+    <col min="13" max="14" width="27.7109375" customWidth="1"/>
+    <col min="15" max="15" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="E2" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
-      <c r="I2" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="M1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="E2" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="I2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
+      <c r="M2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="15"/>
+      <c r="O2" s="16"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="E3" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
-      <c r="I3" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="E3" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="I3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
-      <c r="I4" s="15" t="s">
-        <v>23</v>
+      <c r="E4" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="I4" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="E5" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="I5" s="17"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="E5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="I5" s="44"/>
       <c r="J5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="E7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="E7" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="G7" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="E9" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="44"/>
+      <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="E9" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="1" t="s">
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="E11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="I11" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="E12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="I12" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="E11" s="18" t="s">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="E14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="I14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="E15" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="I11" s="14" t="s">
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="I15" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="E12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="I12" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="E14" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="E15" s="18" t="s">
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="E16" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="F16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16" s="18"/>
+      <c r="K16" s="19"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="E16" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C17" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="28"/>
+        <v>21</v>
+      </c>
+      <c r="E17" s="41"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="18"/>
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="E18" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="I18" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="E19" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="1" t="s">
+      <c r="G19" s="1"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="E18" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="E19" s="30" t="s">
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="43"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="1"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="E22" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="E23" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="E24" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="E22" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="E23" s="34" t="s">
+      <c r="F24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="E24" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="30"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="30"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
+  <mergeCells count="48">
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A16:C16"/>
@@ -1395,18 +1489,23 @@
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E24:E26"/>
     <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Home sweet home ...
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA80C6E-5B02-41AA-81D3-1AFEBBBF2C90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828FD897-0FF4-42D7-9F79-3D0F3F727B65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -280,6 +280,21 @@
   </si>
   <si>
     <t>&lt;Host-Name&gt;/Reports/azargh_feederpeak</t>
+  </si>
+  <si>
+    <t>مازندران ـ اجرای بند اول نامه مطابق توضیحات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Havades_App </t>
+  </si>
+  <si>
+    <t>rptWantedInfo_Mode2.rpt</t>
+  </si>
+  <si>
+    <t>غرب مازندران ـ اضافه شدن فیلتر «نوع موافقت» به گزارش 10-3</t>
+  </si>
+  <si>
+    <t>frmReportHourByHourpower.vb</t>
   </si>
 </sst>
 </file>
@@ -518,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -539,6 +554,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,10 +578,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -573,6 +598,48 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,52 +648,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,46 +988,46 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="E2" s="23" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="E2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
-      <c r="I2" s="14" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
+      <c r="I2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
-      <c r="M2" s="14" t="s">
+      <c r="J2" s="17"/>
+      <c r="K2" s="18"/>
+      <c r="M2" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="16"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="E3" s="26" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="E3" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
-      <c r="I3" s="29" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46"/>
+      <c r="I3" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1014,12 +1035,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
-      <c r="I4" s="20" t="s">
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="I4" s="23" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1028,17 +1049,17 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="E5" s="29" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="E5" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="I5" s="44"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="I5" s="25"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
@@ -1052,24 +1073,24 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="I6" s="44"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="E7" s="20" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="E7" s="23" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1078,11 +1099,11 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -1092,14 +1113,14 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="23" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -1108,24 +1129,24 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="E9" s="22" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="E9" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="I9" s="44"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="I9" s="25"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1141,43 +1162,43 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="44"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="I11" s="29" t="s">
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="I11" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="E12" s="20" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="E12" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="37" t="s">
+      <c r="I12" s="30" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1188,17 +1209,17 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="21"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="39"/>
+      <c r="I13" s="31"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
@@ -1207,38 +1228,38 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-      <c r="I14" s="14" t="s">
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="I14" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="E15" s="22" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="29"/>
+      <c r="E15" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="I15" s="29" t="s">
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="I15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
@@ -1246,7 +1267,7 @@
       </c>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="38" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1255,14 +1276,14 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="19"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1271,29 +1292,29 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="41"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="18"/>
-      <c r="K17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="21"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="I18" s="20" t="s">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="I18" s="23" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1304,19 +1325,19 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="41" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="44"/>
+      <c r="I19" s="25"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1325,17 +1346,17 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="42" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="40" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="44"/>
+      <c r="I20" s="25"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
@@ -1351,10 +1372,10 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="42"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="21"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
@@ -1366,14 +1387,16 @@
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="I22" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
@@ -1381,11 +1404,18 @@
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
+      <c r="I23" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="33"/>
@@ -1393,7 +1423,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="41" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1402,24 +1432,36 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
+      <c r="I24" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="43"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="I25" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="43"/>
+      <c r="E26" s="41"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -1429,15 +1471,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1447,7 +1489,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="21"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1457,12 +1499,34 @@
       <c r="A30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="M3:O3"/>
+  <mergeCells count="49">
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="I3:K3"/>
@@ -1477,35 +1541,14 @@
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="I18:I21"/>
     <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="I2:K2"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
VIEW ViewMonitoringTv Added to SQLs :grin:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828FD897-0FF4-42D7-9F79-3D0F3F727B65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548F91B5-B742-4F9D-81B9-FCF00FFA0C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -295,6 +295,12 @@
   </si>
   <si>
     <t>frmReportHourByHourpower.vb</t>
+  </si>
+  <si>
+    <t>بوشهر ـ تغییر در ویوی مخصوص شرکت الگوریتم پارس به شرح نامه</t>
+  </si>
+  <si>
+    <t>ViewMonitoringTv.sql</t>
   </si>
 </sst>
 </file>
@@ -560,34 +566,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -598,30 +577,45 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -634,19 +628,31 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -931,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,46 +994,48 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="E2" s="27" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="E2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29"/>
-      <c r="I2" s="16" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="I2" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
-      <c r="M2" s="16" t="s">
+      <c r="J2" s="45"/>
+      <c r="K2" s="46"/>
+      <c r="M2" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="17"/>
-      <c r="O2" s="18"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="46"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="E3" s="44" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="E3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46"/>
-      <c r="I3" s="22" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+      <c r="I3" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="M3" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1035,31 +1043,38 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
-      <c r="I4" s="23" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="I4" s="41" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>63</v>
       </c>
       <c r="K4" s="1"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="E5" s="22" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="E5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="I5" s="25"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
@@ -1073,24 +1088,24 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-      <c r="I6" s="25"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="E7" s="23" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="E7" s="41" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1099,11 +1114,11 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -1113,14 +1128,14 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="41" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -1129,24 +1144,24 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="E9" s="26" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="E9" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="I9" s="25"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1162,43 +1177,43 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="25"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="I11" s="22" t="s">
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="I11" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="E12" s="23" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="E12" s="41" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="30" t="s">
+      <c r="I12" s="31" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1209,17 +1224,17 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="24"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="31"/>
+      <c r="I13" s="33"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
@@ -1228,46 +1243,46 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-      <c r="I14" s="16" t="s">
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="I14" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="46"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="E15" s="26" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="E15" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="I15" s="22" t="s">
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="I15" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="E16" s="38" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="E16" s="34" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1276,14 +1291,14 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="40"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="31" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1292,29 +1307,29 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="21"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="40"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="I18" s="23" t="s">
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="I18" s="41" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1325,19 +1340,19 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="37" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="25"/>
+      <c r="I19" s="43"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1346,24 +1361,24 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="40" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="36" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="25"/>
+      <c r="I20" s="43"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="27" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1372,43 +1387,43 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="40"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="36"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="24"/>
+      <c r="I21" s="42"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="I22" s="22" t="s">
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="I22" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="40"/>
       <c r="I23" s="14" t="s">
         <v>86</v>
       </c>
@@ -1418,12 +1433,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="37" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1432,17 +1447,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="41"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -1461,7 +1476,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="41"/>
+      <c r="E26" s="37"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -1471,15 +1486,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="41" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1489,7 +1504,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="24"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1500,33 +1515,12 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="I2:K2"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="I3:K3"/>
@@ -1543,12 +1537,33 @@
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
LoadBalancedReport almost done!!! :truimph::grin:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548F91B5-B742-4F9D-81B9-FCF00FFA0C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DAB896-932D-46D9-9621-601566D8E129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -301,6 +301,27 @@
   </si>
   <si>
     <t>ViewMonitoringTv.sql</t>
+  </si>
+  <si>
+    <t>Report_KHSH_GetLPPostLoadBalance</t>
+  </si>
+  <si>
+    <t>&lt;Host-Name&gt;/Reports/khornorth_lppostloadbalance</t>
+  </si>
+  <si>
+    <t>spGetReport_LPPostLoadBalance</t>
+  </si>
+  <si>
+    <t>KHSH_GetPercentANDLegalCurrent (Function)</t>
+  </si>
+  <si>
+    <t>KHSH_UnbalancedIndicatorA (Function)</t>
+  </si>
+  <si>
+    <t>KHSH_UnbalancedIndicatorB (Function)</t>
+  </si>
+  <si>
+    <t>خراسان شمالی ـ تهیه وب سرویس معادل گزارش تعادل بار</t>
   </si>
 </sst>
 </file>
@@ -539,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -566,7 +587,34 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,6 +625,48 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,75 +676,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,7 +960,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="M7" sqref="M7:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +974,7 @@
     <col min="10" max="10" width="29.28515625" customWidth="1"/>
     <col min="11" max="11" width="35.7109375" customWidth="1"/>
     <col min="13" max="14" width="27.7109375" customWidth="1"/>
-    <col min="15" max="15" width="35.7109375" customWidth="1"/>
+    <col min="15" max="15" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -994,48 +1016,48 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="E2" s="18" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="E2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="I2" s="44" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
+      <c r="I2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="45"/>
-      <c r="K2" s="46"/>
-      <c r="M2" s="44" t="s">
+      <c r="J2" s="17"/>
+      <c r="K2" s="18"/>
+      <c r="M2" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="46"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="E3" s="21" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="E3" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="I3" s="16" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46"/>
+      <c r="I3" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="M3" s="16" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="M3" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1043,12 +1065,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="I4" s="41" t="s">
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="I4" s="23" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1064,21 +1086,26 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="E5" s="16" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="E5" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="I5" s="43"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="I5" s="25"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K5" s="1"/>
+      <c r="M5" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -1088,24 +1115,29 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="40"/>
-      <c r="I6" s="43"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
+      <c r="M6" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="N6" s="20"/>
+      <c r="O6" s="21"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="41" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="E7" s="23" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1114,11 +1146,20 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="M7" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -1128,40 +1169,52 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="23" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="E9" s="17" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="E9" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="I9" s="43"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="I9" s="25"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1177,43 +1230,53 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="43"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="I11" s="16" t="s">
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="I11" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="E12" s="41" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="E12" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="31" t="s">
+      <c r="I12" s="30" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1224,17 +1287,17 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="42"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="33"/>
+      <c r="I13" s="31"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
@@ -1243,46 +1306,46 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
-      <c r="I14" s="44" t="s">
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="I14" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="45"/>
-      <c r="K14" s="46"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="E15" s="17" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="29"/>
+      <c r="E15" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="I15" s="16" t="s">
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="I15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="E16" s="34" t="s">
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="E16" s="38" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1291,14 +1354,14 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="39"/>
-      <c r="K16" s="40"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1307,29 +1370,29 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="38" t="s">
+      <c r="I17" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="21"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="I18" s="41" t="s">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="I18" s="23" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1340,19 +1403,19 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="41" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="43"/>
+      <c r="I19" s="25"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1361,24 +1424,24 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="36" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="40" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="43"/>
+      <c r="I20" s="25"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1387,43 +1450,43 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="36"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="42"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="I22" s="16" t="s">
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="I22" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="40"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
       <c r="I23" s="14" t="s">
         <v>86</v>
       </c>
@@ -1433,12 +1496,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="37" t="s">
+      <c r="E24" s="41" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1447,17 +1510,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="16" t="s">
+      <c r="I24" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="37"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -1476,7 +1539,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="37"/>
+      <c r="E26" s="41"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -1486,15 +1549,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="41" t="s">
+      <c r="E28" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1504,7 +1567,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="42"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1514,13 +1577,34 @@
       <c r="A30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="I2:K2"/>
+  <mergeCells count="52">
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="I3:K3"/>
@@ -1537,33 +1621,15 @@
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:M11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Make sure it's updated :smiley:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7913EE-F64F-473A-B1D3-9AB57602AB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC45187-2D2C-4983-993E-5B0170BD12CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Spring" sheetId="1" r:id="rId1"/>
+    <sheet name="Summer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="112">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -267,9 +268,6 @@
     <t>spGetReport_PostFeederLoad</t>
   </si>
   <si>
-    <t>8th Week (1400/2/07)</t>
-  </si>
-  <si>
     <t>7th Week (1400/3/1)</t>
   </si>
   <si>
@@ -322,13 +320,77 @@
   </si>
   <si>
     <t>خراسان شمالی ـ تهیه وب سرویس معادل گزارش تعادل بار</t>
+  </si>
+  <si>
+    <t>توانیر ـ تهیه گزارش درخواستی در نرم افزار رصد</t>
+  </si>
+  <si>
+    <t>Tavanir_App</t>
+  </si>
+  <si>
+    <t>frmMonitoring.vb</t>
+  </si>
+  <si>
+    <t>frmReportDisHourly.vb</t>
+  </si>
+  <si>
+    <r>
+      <t>spReportHourlyDisconnectPower (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AbediNejad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>8th Week (1400/3/08)</t>
+  </si>
+  <si>
+    <t>&lt;Host-Name&gt;/NewTamirRequest/Maz_SetRequestTamir</t>
+  </si>
+  <si>
+    <t>مازندران ـ ایجاد وب سرویس ثبت درخواست اولیه خاموشی بابرنامه ـ بخش اول</t>
+  </si>
+  <si>
+    <t>Global.asax.cs</t>
+  </si>
+  <si>
+    <t>AddNewTamirRequest.aspx</t>
+  </si>
+  <si>
+    <t>HavadesTamir.asmx.cs</t>
+  </si>
+  <si>
+    <t>9th Week (1400/3/15)</t>
+  </si>
+  <si>
+    <t>10th Week (1400/3/22)</t>
+  </si>
+  <si>
+    <t>13th Week (1400/4/05)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +429,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -560,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -588,7 +657,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -599,6 +704,48 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,75 +753,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -957,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,11 +1053,13 @@
     <col min="11" max="11" width="35.7109375" customWidth="1"/>
     <col min="13" max="14" width="27.7109375" customWidth="1"/>
     <col min="15" max="15" width="43.140625" customWidth="1"/>
+    <col min="17" max="18" width="27.7109375" customWidth="1"/>
+    <col min="19" max="19" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -988,7 +1068,7 @@
         <v>62</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
@@ -997,7 +1077,7 @@
         <v>62</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>5</v>
@@ -1006,7 +1086,7 @@
         <v>62</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>5</v>
@@ -1014,63 +1094,80 @@
       <c r="O1" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="E2" s="19" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="I2" s="45" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
+      <c r="I2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="47"/>
-      <c r="M2" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="47"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="J2" s="25"/>
+      <c r="K2" s="26"/>
+      <c r="M2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="25"/>
+      <c r="O2" s="26"/>
+      <c r="Q2" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="R2" s="25"/>
+      <c r="S2" s="26"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="E3" s="22" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="E3" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
-      <c r="I3" s="17" t="s">
+      <c r="F3" s="49"/>
+      <c r="G3" s="50"/>
+      <c r="I3" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="M3" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="M3" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="I4" s="42" t="s">
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="I4" s="27" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1082,32 +1179,32 @@
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="E5" s="17" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="E5" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="I5" s="44"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M5" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -1115,29 +1212,29 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
-      <c r="I6" s="44"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="20"/>
+      <c r="I6" s="29"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="N6" s="40"/>
-      <c r="O6" s="41"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="M6" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" s="36"/>
+      <c r="O6" s="20"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="E7" s="42" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="E7" s="27" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1146,22 +1243,22 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="M7" s="38" t="s">
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="M7" s="21" t="s">
         <v>34</v>
       </c>
       <c r="N7" s="16" t="s">
         <v>37</v>
       </c>
       <c r="O7" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -1169,52 +1266,52 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="27" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="38"/>
+      <c r="M8" s="21"/>
       <c r="N8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="E9" s="18" t="s">
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="E9" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="I9" s="44"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="I9" s="29"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="38"/>
+      <c r="M9" s="21"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1230,53 +1327,53 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="44"/>
+      <c r="I10" s="29"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="38"/>
+      <c r="M10" s="21"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="I11" s="17" t="s">
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="I11" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="M11" s="38"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="M11" s="21"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="E12" s="42" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="E12" s="27" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="32" t="s">
+      <c r="I12" s="34" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1285,67 +1382,91 @@
       <c r="K12" s="12" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="M12" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="43"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="34"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="M13" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
-      <c r="I14" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="J14" s="46"/>
-      <c r="K14" s="47"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+      <c r="I14" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="E15" s="18" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="E15" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="I15" s="17" t="s">
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="I15" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="M15" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="N15" s="25"/>
+      <c r="O15" s="26"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
-      <c r="E16" s="35" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="E16" s="43" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1354,14 +1475,19 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="I16" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="36"/>
+      <c r="K16" s="20"/>
+      <c r="M16" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1370,29 +1496,34 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="36"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
-    </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+      <c r="I17" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" s="36"/>
+      <c r="K17" s="20"/>
+      <c r="M17" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="N17" s="19"/>
+      <c r="O17" s="20"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="42"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="I18" s="42" t="s">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="I18" s="27" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1401,47 +1532,64 @@
       <c r="K18" s="13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+      <c r="M18" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="21" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="44"/>
+      <c r="I19" s="29"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="M19" s="21"/>
+      <c r="N19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="37" t="s">
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="45" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="44"/>
+      <c r="I20" s="29"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="M20" s="21"/>
+      <c r="N20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1450,58 +1598,60 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="37"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="43"/>
+      <c r="I21" s="28"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+      <c r="M21" s="17"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="I22" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="I22" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="M22" s="17"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="38"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="40"/>
-      <c r="G23" s="41"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="38"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="21" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1510,17 +1660,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I24" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="38"/>
+      <c r="E25" s="21"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -1528,36 +1678,36 @@
         <v>59</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="38"/>
+      <c r="E26" s="21"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="42" t="s">
+      <c r="E28" s="27" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1565,19 +1715,27 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="43"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="60">
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="I17:K17"/>
@@ -1586,7 +1744,27 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="I3:K3"/>
@@ -1603,35 +1781,87 @@
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A23382B-C91E-4BC1-BA64-857291C2DF07}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New Sp is Fucking me :weary:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB158C69-802D-4CE0-B212-C0EFA60E3D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55C331C-BD4F-4A8A-887C-EF8D01C15F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -731,25 +731,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -759,15 +740,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -778,33 +751,54 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -814,19 +808,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1117,7 +1117,7 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="Q12" sqref="Q12:S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,58 +1184,58 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="E2" s="35" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="E2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37"/>
-      <c r="I2" s="28" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="I2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
-      <c r="M2" s="28" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
+      <c r="M2" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
-      <c r="Q2" s="28" t="s">
+      <c r="N2" s="22"/>
+      <c r="O2" s="23"/>
+      <c r="Q2" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="30"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="23"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="E3" s="52" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="E3" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
-      <c r="I3" s="21" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="I3" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="M3" s="21" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="M3" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="Q3" s="21" t="s">
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="Q3" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1243,12 +1243,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
-      <c r="I4" s="31" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="I4" s="49" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1262,7 +1262,7 @@
       <c r="O4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="22" t="s">
+      <c r="Q4" s="52" t="s">
         <v>99</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1271,27 +1271,27 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="E5" s="21" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="E5" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="I5" s="33"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="Q5" s="22"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="12" t="s">
         <v>113</v>
       </c>
@@ -1305,34 +1305,34 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="26"/>
-      <c r="I6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="24" t="s">
+      <c r="M6" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="40"/>
-      <c r="O6" s="26"/>
-      <c r="Q6" s="22"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="34"/>
+      <c r="Q6" s="52"/>
       <c r="R6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="E7" s="31" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="E7" s="49" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1341,12 +1341,12 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="M7" s="27" t="s">
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="M7" s="48" t="s">
         <v>34</v>
       </c>
       <c r="N7" s="16" t="s">
@@ -1355,7 +1355,7 @@
       <c r="O7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="22"/>
+      <c r="Q7" s="52"/>
       <c r="R7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1369,62 +1369,62 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="49" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="27"/>
+      <c r="M8" s="48"/>
       <c r="N8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="22"/>
+      <c r="Q8" s="52"/>
       <c r="R8" s="1" t="s">
         <v>116</v>
       </c>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="E9" s="34" t="s">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="E9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="I9" s="33"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="I9" s="51"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="27"/>
+      <c r="M9" s="48"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="Q9" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1440,12 +1440,12 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="33"/>
+      <c r="I10" s="51"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="27"/>
+      <c r="M10" s="48"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
         <v>95</v>
@@ -1461,46 +1461,46 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="I11" s="21" t="s">
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="I11" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="M11" s="27"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="M11" s="48"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q11" s="23" t="s">
+      <c r="Q11" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="E12" s="31" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="E12" s="49" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="42" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1509,36 +1509,36 @@
       <c r="K12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="M12" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="Q12" s="21" t="s">
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="Q12" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="32"/>
+      <c r="E13" s="50"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="39"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="22" t="s">
+      <c r="M13" s="52" t="s">
         <v>99</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1547,7 +1547,7 @@
       <c r="O13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q13" s="27" t="s">
+      <c r="Q13" s="48" t="s">
         <v>55</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1556,61 +1556,61 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
-      <c r="I14" s="28" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="I14" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30"/>
-      <c r="M14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
+      <c r="M14" s="52"/>
       <c r="N14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="Q14" s="27"/>
+      <c r="Q14" s="48"/>
       <c r="R14" s="1" t="s">
         <v>123</v>
       </c>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="E15" s="34" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="E15" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="I15" s="21" t="s">
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="I15" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="M15" s="28" t="s">
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="M15" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="29"/>
-      <c r="O15" s="30"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="23"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="E16" s="47" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="E16" s="45" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1619,19 +1619,19 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="40"/>
-      <c r="K16" s="26"/>
-      <c r="M16" s="21" t="s">
+      <c r="J16" s="33"/>
+      <c r="K16" s="34"/>
+      <c r="M16" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="42" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1640,34 +1640,34 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="48"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="40"/>
-      <c r="K17" s="26"/>
-      <c r="M17" s="24" t="s">
+      <c r="J17" s="33"/>
+      <c r="K17" s="34"/>
+      <c r="M17" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="25"/>
-      <c r="O17" s="26"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="34"/>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="I18" s="31" t="s">
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="I18" s="49" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1676,7 +1676,7 @@
       <c r="K18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="27" t="s">
+      <c r="M18" s="48" t="s">
         <v>34</v>
       </c>
       <c r="N18" s="1" t="s">
@@ -1685,55 +1685,55 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="48" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="33"/>
+      <c r="I19" s="51"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="27"/>
+      <c r="M19" s="48"/>
       <c r="N19" s="1" t="s">
         <v>107</v>
       </c>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="49" t="s">
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="47" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="33"/>
+      <c r="I20" s="51"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="27"/>
+      <c r="M20" s="48"/>
       <c r="N20" s="1" t="s">
         <v>108</v>
       </c>
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="38" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1742,10 +1742,10 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="49"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="47"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="32"/>
+      <c r="I21" s="50"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
@@ -1753,34 +1753,34 @@
       <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="I22" s="21" t="s">
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="I22" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="40"/>
-      <c r="G23" s="26"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34"/>
       <c r="I23" s="14" t="s">
         <v>85</v>
       </c>
@@ -1790,12 +1790,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="48" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1804,17 +1804,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="27"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -1833,7 +1833,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="27"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -1843,15 +1843,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="49" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1861,7 +1861,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="32"/>
+      <c r="E29" s="50"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1872,6 +1872,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q4:Q8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="I24:K24"/>
@@ -1888,55 +1937,6 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q4:Q8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="Q13:Q14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1969,38 +1969,38 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="48" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>

</xml_diff>

<commit_message>
Report 10-4 added to Fucking Software HavadesApp
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55C331C-BD4F-4A8A-887C-EF8D01C15F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5808716-A4AE-4A82-B12D-B06D7624F526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="130">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -439,6 +439,21 @@
   </si>
   <si>
     <t>12th Week (1400/4/05)</t>
+  </si>
+  <si>
+    <t>Report_10_4</t>
+  </si>
+  <si>
+    <t>spDisHourly_Daily</t>
+  </si>
+  <si>
+    <t>Report_10_4_DisHourly.mrt</t>
+  </si>
+  <si>
+    <t>frmReportDisHourByHour.vb</t>
+  </si>
+  <si>
+    <t>جنوب کرمان ـ ایجاد گزارش جدید انرژی توزیع نشده ساعت به ساعت به شرح توضیحات</t>
   </si>
 </sst>
 </file>
@@ -731,6 +746,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -740,7 +774,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -751,6 +793,48 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -758,75 +842,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1117,7 +1132,7 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12:S12"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,58 +1199,58 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="E2" s="26" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="E2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
-      <c r="I2" s="21" t="s">
+      <c r="F2" s="36"/>
+      <c r="G2" s="37"/>
+      <c r="I2" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="23"/>
-      <c r="M2" s="21" t="s">
+      <c r="J2" s="29"/>
+      <c r="K2" s="30"/>
+      <c r="M2" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="22"/>
-      <c r="O2" s="23"/>
-      <c r="Q2" s="21" t="s">
+      <c r="N2" s="29"/>
+      <c r="O2" s="30"/>
+      <c r="Q2" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="R2" s="22"/>
-      <c r="S2" s="23"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="30"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="E3" s="29" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="E3" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
-      <c r="I3" s="24" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="54"/>
+      <c r="I3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="M3" s="24" t="s">
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="M3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="Q3" s="24" t="s">
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="Q3" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1243,12 +1258,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="I4" s="49" t="s">
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
+      <c r="I4" s="31" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1262,7 +1277,7 @@
       <c r="O4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="22" t="s">
         <v>99</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1271,27 +1286,27 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="E5" s="24" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="E5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="I5" s="51"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="I5" s="33"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="Q5" s="52"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="Q5" s="22"/>
       <c r="R5" s="12" t="s">
         <v>113</v>
       </c>
@@ -1305,34 +1320,34 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
-      <c r="I6" s="51"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="26"/>
+      <c r="I6" s="33"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="33"/>
-      <c r="O6" s="34"/>
-      <c r="Q6" s="52"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="26"/>
+      <c r="Q6" s="22"/>
       <c r="R6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="E7" s="49" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="E7" s="31" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1341,12 +1356,12 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="M7" s="48" t="s">
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="M7" s="27" t="s">
         <v>34</v>
       </c>
       <c r="N7" s="16" t="s">
@@ -1355,7 +1370,7 @@
       <c r="O7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="52"/>
+      <c r="Q7" s="22"/>
       <c r="R7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1369,62 +1384,62 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="50"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="49" t="s">
+      <c r="I8" s="31" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="48"/>
+      <c r="M8" s="27"/>
       <c r="N8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="52"/>
+      <c r="Q8" s="22"/>
       <c r="R8" s="1" t="s">
         <v>116</v>
       </c>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="E9" s="25" t="s">
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="E9" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="I9" s="51"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="I9" s="33"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="48"/>
+      <c r="M9" s="27"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q9" s="24" t="s">
+      <c r="Q9" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1440,12 +1455,12 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="51"/>
+      <c r="I10" s="33"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="48"/>
+      <c r="M10" s="27"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
         <v>95</v>
@@ -1461,46 +1476,46 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="I11" s="24" t="s">
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="I11" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="M11" s="48"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="M11" s="27"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q11" s="53" t="s">
+      <c r="Q11" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="53"/>
-      <c r="S11" s="53"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="E12" s="49" t="s">
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="E12" s="31" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="42" t="s">
+      <c r="I12" s="38" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1509,36 +1524,36 @@
       <c r="K12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="M12" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="Q12" s="24" t="s">
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="Q12" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="50"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="44"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="52" t="s">
+      <c r="M13" s="22" t="s">
         <v>99</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1547,7 +1562,7 @@
       <c r="O13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q13" s="48" t="s">
+      <c r="Q13" s="27" t="s">
         <v>55</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1556,61 +1571,66 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="I14" s="21" t="s">
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="I14" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="23"/>
-      <c r="M14" s="52"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="30"/>
+      <c r="M14" s="22"/>
       <c r="N14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="Q14" s="48"/>
+      <c r="Q14" s="27"/>
       <c r="R14" s="1" t="s">
         <v>123</v>
       </c>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="E15" s="25" t="s">
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="E15" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="I15" s="24" t="s">
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="I15" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="M15" s="21" t="s">
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="M15" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="22"/>
-      <c r="O15" s="23"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="30"/>
+      <c r="Q15" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
-      <c r="E16" s="45" t="s">
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="E16" s="47" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1619,19 +1639,28 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="32" t="s">
+      <c r="I16" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="34"/>
-      <c r="M16" s="24" t="s">
+      <c r="J16" s="40"/>
+      <c r="K16" s="26"/>
+      <c r="M16" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-    </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="Q16" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S16" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1640,34 +1669,41 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="46"/>
+      <c r="E17" s="48"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="32" t="s">
+      <c r="I17" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="34"/>
-      <c r="M17" s="32" t="s">
+      <c r="J17" s="40"/>
+      <c r="K17" s="26"/>
+      <c r="M17" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="54"/>
-      <c r="O17" s="34"/>
-    </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="26"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="46"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="I18" s="49" t="s">
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="I18" s="31" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1676,64 +1712,67 @@
       <c r="K18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="48" t="s">
+      <c r="M18" s="27" t="s">
         <v>34</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="27" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="51"/>
+      <c r="I19" s="33"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="48"/>
+      <c r="M19" s="27"/>
       <c r="N19" s="1" t="s">
         <v>107</v>
       </c>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="47" t="s">
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="49" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="51"/>
+      <c r="I20" s="33"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="48"/>
+      <c r="M20" s="27"/>
       <c r="N20" s="1" t="s">
         <v>108</v>
       </c>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1742,45 +1781,45 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="48"/>
-      <c r="F21" s="47"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="49"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="50"/>
+      <c r="I21" s="32"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M21" s="17"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="I22" s="24" t="s">
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="I22" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
       <c r="M22" s="17"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="34"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="26"/>
       <c r="I23" s="14" t="s">
         <v>85</v>
       </c>
@@ -1789,13 +1828,13 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="27" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1804,17 +1843,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="24" t="s">
+      <c r="I24" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="48"/>
+      <c r="E25" s="27"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -1829,29 +1868,29 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="48"/>
+      <c r="E26" s="27"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="49" t="s">
+      <c r="E28" s="31" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1859,31 +1898,56 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="50"/>
+      <c r="E29" s="32"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q4:Q8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
+  <mergeCells count="68">
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="I3:K3"/>
@@ -1900,43 +1964,21 @@
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q4:Q8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="Q18:S18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1969,38 +2011,38 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="34"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>

</xml_diff>

<commit_message>
Some changes in data gathering :weary:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5808716-A4AE-4A82-B12D-B06D7624F526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41588A6D-FE61-4880-8618-5BC628A8720F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="130">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -746,25 +746,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -774,15 +755,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -793,33 +766,54 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -829,19 +823,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1131,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="N7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,58 +1199,58 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="E2" s="35" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="E2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37"/>
-      <c r="I2" s="28" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="I2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
-      <c r="M2" s="28" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
+      <c r="M2" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
-      <c r="Q2" s="28" t="s">
+      <c r="N2" s="22"/>
+      <c r="O2" s="23"/>
+      <c r="Q2" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="30"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="23"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="E3" s="52" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="E3" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
-      <c r="I3" s="21" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="I3" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="M3" s="21" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="M3" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="Q3" s="21" t="s">
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="Q3" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1258,12 +1258,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
-      <c r="I4" s="31" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="I4" s="49" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1277,7 +1277,7 @@
       <c r="O4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="22" t="s">
+      <c r="Q4" s="52" t="s">
         <v>99</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1286,27 +1286,27 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="E5" s="21" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="E5" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="I5" s="33"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="Q5" s="22"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="12" t="s">
         <v>113</v>
       </c>
@@ -1320,34 +1320,34 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="26"/>
-      <c r="I6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="24" t="s">
+      <c r="M6" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="40"/>
-      <c r="O6" s="26"/>
-      <c r="Q6" s="22"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="34"/>
+      <c r="Q6" s="52"/>
       <c r="R6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="E7" s="31" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="E7" s="49" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1356,12 +1356,12 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="M7" s="27" t="s">
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="M7" s="48" t="s">
         <v>34</v>
       </c>
       <c r="N7" s="16" t="s">
@@ -1370,7 +1370,7 @@
       <c r="O7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="22"/>
+      <c r="Q7" s="52"/>
       <c r="R7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1384,62 +1384,62 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="49" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="27"/>
+      <c r="M8" s="48"/>
       <c r="N8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="22"/>
+      <c r="Q8" s="52"/>
       <c r="R8" s="1" t="s">
         <v>116</v>
       </c>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="E9" s="34" t="s">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="E9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="I9" s="33"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="I9" s="51"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="27"/>
+      <c r="M9" s="48"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="Q9" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1455,12 +1455,12 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="33"/>
+      <c r="I10" s="51"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="27"/>
+      <c r="M10" s="48"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
         <v>95</v>
@@ -1476,46 +1476,46 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="I11" s="21" t="s">
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="I11" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="M11" s="27"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="M11" s="48"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q11" s="23" t="s">
+      <c r="Q11" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="E12" s="31" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="E12" s="49" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="42" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1524,36 +1524,36 @@
       <c r="K12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="M12" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="Q12" s="21" t="s">
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="Q12" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="32"/>
+      <c r="E13" s="50"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="39"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="22" t="s">
+      <c r="M13" s="52" t="s">
         <v>99</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1562,7 +1562,7 @@
       <c r="O13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q13" s="27" t="s">
+      <c r="Q13" s="48" t="s">
         <v>55</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1571,66 +1571,66 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
-      <c r="I14" s="28" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="I14" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30"/>
-      <c r="M14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
+      <c r="M14" s="52"/>
       <c r="N14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="Q14" s="27"/>
+      <c r="Q14" s="48"/>
       <c r="R14" s="1" t="s">
         <v>123</v>
       </c>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="E15" s="34" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="E15" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="I15" s="21" t="s">
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="I15" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="M15" s="28" t="s">
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="M15" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="29"/>
-      <c r="O15" s="30"/>
-      <c r="Q15" s="21" t="s">
+      <c r="N15" s="22"/>
+      <c r="O15" s="23"/>
+      <c r="Q15" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="E16" s="47" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="E16" s="45" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1639,18 +1639,18 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="40"/>
-      <c r="K16" s="26"/>
-      <c r="M16" s="21" t="s">
+      <c r="J16" s="33"/>
+      <c r="K16" s="34"/>
+      <c r="M16" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="Q16" s="31" t="s">
-        <v>55</v>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="Q16" s="52" t="s">
+        <v>22</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>127</v>
@@ -1660,7 +1660,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="42" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1669,41 +1669,41 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="48"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="40"/>
-      <c r="K17" s="26"/>
-      <c r="M17" s="24" t="s">
+      <c r="J17" s="33"/>
+      <c r="K17" s="34"/>
+      <c r="M17" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="25"/>
-      <c r="O17" s="26"/>
-      <c r="Q17" s="33"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="34"/>
+      <c r="Q17" s="52"/>
       <c r="R17" s="1" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="I18" s="31" t="s">
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="I18" s="49" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1712,67 +1712,69 @@
       <c r="K18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="27" t="s">
+      <c r="M18" s="48" t="s">
         <v>34</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="48" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="33"/>
+      <c r="I19" s="51"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="27"/>
+      <c r="M19" s="48"/>
       <c r="N19" s="1" t="s">
         <v>107</v>
       </c>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="49" t="s">
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="47" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="33"/>
+      <c r="I20" s="51"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="27"/>
+      <c r="M20" s="48"/>
       <c r="N20" s="1" t="s">
         <v>108</v>
       </c>
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="38" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1781,10 +1783,10 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="49"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="47"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="32"/>
+      <c r="I21" s="50"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
@@ -1792,34 +1794,34 @@
       <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="I22" s="21" t="s">
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="I22" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="40"/>
-      <c r="G23" s="26"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34"/>
       <c r="I23" s="14" t="s">
         <v>85</v>
       </c>
@@ -1829,12 +1831,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="48" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1843,17 +1845,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="27"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -1872,7 +1874,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="27"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -1882,15 +1884,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="49" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1900,7 +1902,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="32"/>
+      <c r="E29" s="50"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1910,7 +1912,58 @@
       <c r="A30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="68">
+  <mergeCells count="67">
+    <mergeCell ref="Q16:Q18"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q4:Q8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="I24:K24"/>
@@ -1927,58 +1980,6 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q4:Q8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="Q18:S18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2011,38 +2012,38 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="48" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>

</xml_diff>

<commit_message>
Spin that shit :wink:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB603F8-8A4A-4FEA-9524-850971373176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3264C6E4-53C3-4D35-8BD0-3FE40FEC2AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="135">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -458,12 +458,24 @@
   <si>
     <t>ایلام ـ انجام بندهای 2 و 4 نامه پیوست</t>
   </si>
+  <si>
+    <t>HInforms.aspx</t>
+  </si>
+  <si>
+    <t>HavadesInform.asmx</t>
+  </si>
+  <si>
+    <t>البرز ـ تغییر در وب سرویسهای مورد نظر جهت ایجاد امکان جستجوی خاموشی‌ها بر اساس شناسه قبض، آدرس، شماره موبایل و تاریخ خاموشی</t>
+  </si>
+  <si>
+    <t>&lt;Host-Name&gt;/Inform/GetSubscriberOutageListbyBillMob</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +535,13 @@
       <color rgb="FFFF0000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -713,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -752,25 +771,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -780,15 +780,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -799,33 +791,54 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -835,22 +848,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,7 +1158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="N4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" view="pageBreakPreview" topLeftCell="L5" zoomScale="87" zoomScaleNormal="100" zoomScaleSheetLayoutView="87" workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15:S15"/>
     </sheetView>
   </sheetViews>
@@ -1206,58 +1226,58 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="E2" s="36" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="E2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="I2" s="29" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
+      <c r="I2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
-      <c r="M2" s="29" t="s">
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
+      <c r="M2" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
-      <c r="Q2" s="29" t="s">
+      <c r="N2" s="23"/>
+      <c r="O2" s="24"/>
+      <c r="Q2" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="31"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="24"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="E3" s="53" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="E3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55"/>
-      <c r="I3" s="23" t="s">
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
+      <c r="I3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="M3" s="23" t="s">
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="M3" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="Q3" s="23" t="s">
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="Q3" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1265,12 +1285,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
-      <c r="I4" s="32" t="s">
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="I4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1284,7 +1304,7 @@
       <c r="O4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="22" t="s">
+      <c r="Q4" s="54" t="s">
         <v>99</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1293,27 +1313,27 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="E5" s="23" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="E5" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="I5" s="34"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="Q5" s="22"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="Q5" s="54"/>
       <c r="R5" s="12" t="s">
         <v>113</v>
       </c>
@@ -1327,34 +1347,34 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="27"/>
-      <c r="I6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="35"/>
+      <c r="I6" s="52"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="41"/>
-      <c r="O6" s="27"/>
-      <c r="Q6" s="22"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="35"/>
+      <c r="Q6" s="54"/>
       <c r="R6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="E7" s="32" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="E7" s="50" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1363,12 +1383,12 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="M7" s="28" t="s">
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="M7" s="49" t="s">
         <v>34</v>
       </c>
       <c r="N7" s="16" t="s">
@@ -1377,7 +1397,7 @@
       <c r="O7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="22"/>
+      <c r="Q7" s="54"/>
       <c r="R7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1391,62 +1411,62 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="33"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="50" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="28"/>
+      <c r="M8" s="49"/>
       <c r="N8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="22"/>
+      <c r="Q8" s="54"/>
       <c r="R8" s="1" t="s">
         <v>116</v>
       </c>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="E9" s="35" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="E9" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="I9" s="34"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="I9" s="52"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="28"/>
+      <c r="M9" s="49"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q9" s="23" t="s">
+      <c r="Q9" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1462,12 +1482,12 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="34"/>
+      <c r="I10" s="52"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="28"/>
+      <c r="M10" s="49"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
         <v>95</v>
@@ -1483,46 +1503,46 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="I11" s="23" t="s">
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="I11" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="M11" s="28"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="M11" s="49"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q11" s="24" t="s">
+      <c r="Q11" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
+      <c r="R11" s="56"/>
+      <c r="S11" s="56"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="E12" s="32" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="E12" s="50" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="43" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1531,36 +1551,36 @@
       <c r="K12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="Q12" s="23" t="s">
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="Q12" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="33"/>
+      <c r="E13" s="51"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="40"/>
+      <c r="I13" s="45"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="22" t="s">
+      <c r="M13" s="54" t="s">
         <v>99</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1569,7 +1589,7 @@
       <c r="O13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q13" s="28" t="s">
+      <c r="Q13" s="49" t="s">
         <v>55</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1578,66 +1598,66 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
-      <c r="I14" s="29" t="s">
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="I14" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="31"/>
-      <c r="M14" s="22"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
+      <c r="M14" s="54"/>
       <c r="N14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="Q14" s="28"/>
+      <c r="Q14" s="49"/>
       <c r="R14" s="1" t="s">
         <v>123</v>
       </c>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="E15" s="35" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="29"/>
+      <c r="E15" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="I15" s="23" t="s">
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="I15" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="M15" s="29" t="s">
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="M15" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="30"/>
-      <c r="O15" s="31"/>
-      <c r="Q15" s="23" t="s">
+      <c r="N15" s="23"/>
+      <c r="O15" s="24"/>
+      <c r="Q15" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="E16" s="48" t="s">
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="E16" s="46" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1646,17 +1666,17 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="41"/>
-      <c r="K16" s="27"/>
-      <c r="M16" s="23" t="s">
+      <c r="J16" s="34"/>
+      <c r="K16" s="35"/>
+      <c r="M16" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="Q16" s="22" t="s">
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="Q16" s="54" t="s">
         <v>22</v>
       </c>
       <c r="R16" s="1" t="s">
@@ -1667,7 +1687,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="43" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1676,22 +1696,22 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="49"/>
+      <c r="E17" s="47"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="I17" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="41"/>
-      <c r="K17" s="27"/>
-      <c r="M17" s="25" t="s">
+      <c r="J17" s="34"/>
+      <c r="K17" s="35"/>
+      <c r="M17" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="27"/>
-      <c r="Q17" s="22"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="35"/>
+      <c r="Q17" s="54"/>
       <c r="R17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1700,17 +1720,17 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="I18" s="32" t="s">
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="I18" s="50" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1719,67 +1739,67 @@
       <c r="K18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="28" t="s">
+      <c r="M18" s="49" t="s">
         <v>34</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="Q18" s="22"/>
+      <c r="Q18" s="54"/>
       <c r="R18" s="1" t="s">
         <v>128</v>
       </c>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="49" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="34"/>
+      <c r="I19" s="52"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="28"/>
+      <c r="M19" s="49"/>
       <c r="N19" s="1" t="s">
         <v>107</v>
       </c>
       <c r="O19" s="1"/>
-      <c r="Q19" s="23" t="s">
+      <c r="Q19" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="50" t="s">
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="48" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="34"/>
+      <c r="I20" s="52"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="28"/>
+      <c r="M20" s="49"/>
       <c r="N20" s="1" t="s">
         <v>108</v>
       </c>
@@ -1795,7 +1815,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="39" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1804,48 +1824,48 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="50"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="48"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="33"/>
+      <c r="I21" s="51"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M21" s="17"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="55"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="I22" s="23" t="s">
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="I22" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="27"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="35"/>
       <c r="I23" s="14" t="s">
         <v>85</v>
       </c>
@@ -1855,12 +1875,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="49" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1869,17 +1889,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="28"/>
+      <c r="E25" s="49"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -1898,7 +1918,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="28"/>
+      <c r="E26" s="49"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -1908,15 +1928,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="32" t="s">
+      <c r="E28" s="50" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1926,7 +1946,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="33"/>
+      <c r="E29" s="51"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1937,6 +1957,59 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q16:Q18"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q4:Q8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="I24:K24"/>
@@ -1953,59 +2026,6 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q16:Q18"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q4:Q8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q11:S11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2016,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A23382B-C91E-4BC1-BA64-857291C2DF07}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2038,48 +2058,56 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="A3" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="35"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fill my Excel Data :wink:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3264C6E4-53C3-4D35-8BD0-3FE40FEC2AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53C3C36-39D5-49E9-A605-6EB2F2B2FA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="171">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -469,6 +469,114 @@
   </si>
   <si>
     <t>&lt;Host-Name&gt;/Inform/GetSubscriberOutageListbyBillMob</t>
+  </si>
+  <si>
+    <t>ایلام ـ اضافه شدن فیلتر خط گرم به گزارشات سرویس و اضافه شدن «تجهیزات مصرف شده» به گزارش کلی تجعمی 6-2</t>
+  </si>
+  <si>
+    <t>Bazdid_App</t>
+  </si>
+  <si>
+    <t>frmMakeReports.vb</t>
+  </si>
+  <si>
+    <t>spGetReport_2_1_1</t>
+  </si>
+  <si>
+    <t>spGetReport_2_1_2</t>
+  </si>
+  <si>
+    <t>spGetReport_2_1_5</t>
+  </si>
+  <si>
+    <t>spGetReport_2_1_8</t>
+  </si>
+  <si>
+    <t>spGetReport_2_2_1</t>
+  </si>
+  <si>
+    <t>spGetReport_2_2_2</t>
+  </si>
+  <si>
+    <t>spGetReport_2_2_5</t>
+  </si>
+  <si>
+    <t>spGetReport_2_2_6</t>
+  </si>
+  <si>
+    <t>spGetReport_2_2_8</t>
+  </si>
+  <si>
+    <t>spGetReport_2_3_8</t>
+  </si>
+  <si>
+    <t>spGetReport_2_34_1</t>
+  </si>
+  <si>
+    <t>spGetReport_2_34_2</t>
+  </si>
+  <si>
+    <t>spGetReport_2_34_5</t>
+  </si>
+  <si>
+    <t>spGetReport_2_34_6</t>
+  </si>
+  <si>
+    <t>13th Week (1400/4/12)</t>
+  </si>
+  <si>
+    <t>Bargh_GIS</t>
+  </si>
+  <si>
+    <t>TraceMap</t>
+  </si>
+  <si>
+    <t>Report 2_@_@</t>
+  </si>
+  <si>
+    <t>spTraceArea</t>
+  </si>
+  <si>
+    <t>spTraceMaster</t>
+  </si>
+  <si>
+    <t>spTraceTablet</t>
+  </si>
+  <si>
+    <t>spGetStateTrace</t>
+  </si>
+  <si>
+    <t>spOnCallInfo</t>
+  </si>
+  <si>
+    <t>spTraceInfo*</t>
+  </si>
+  <si>
+    <t>spTraceOnCall</t>
+  </si>
+  <si>
+    <t>spTraceRequest</t>
+  </si>
+  <si>
+    <t>TaravMapUC_Cars.xampl.cs</t>
+  </si>
+  <si>
+    <t>Bargh_GIS.csproj</t>
+  </si>
+  <si>
+    <t>[Havades_App] frmMain.vb</t>
+  </si>
+  <si>
+    <t>[Havades_App] ModuleToolAMB.vb</t>
+  </si>
+  <si>
+    <t>frmTraceHistory.cs</t>
+  </si>
+  <si>
+    <t>frmTraceHistoryUI.cs</t>
+  </si>
+  <si>
+    <t>داخلی ـ کار روی تکمیل سازی نقشه طرح هما در نرم افزار ویندوزی Map</t>
   </si>
 </sst>
 </file>
@@ -544,7 +652,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -596,6 +704,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -771,6 +885,27 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -780,7 +915,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -791,6 +934,48 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,77 +985,20 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1158,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" view="pageBreakPreview" topLeftCell="L5" zoomScale="87" zoomScaleNormal="100" zoomScaleSheetLayoutView="87" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15:S15"/>
+    <sheetView rightToLeft="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,31 +1354,31 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="E2" s="27" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="E2" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29"/>
-      <c r="I2" s="22" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="I2" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="24"/>
-      <c r="M2" s="22" t="s">
+      <c r="J2" s="32"/>
+      <c r="K2" s="33"/>
+      <c r="M2" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="24"/>
-      <c r="Q2" s="22" t="s">
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
+      <c r="Q2" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="R2" s="23"/>
-      <c r="S2" s="24"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="33"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
@@ -1258,11 +1386,11 @@
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="57"/>
       <c r="I3" s="25" t="s">
         <v>65</v>
       </c>
@@ -1285,12 +1413,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
-      <c r="I4" s="50" t="s">
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="I4" s="34" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1304,7 +1432,7 @@
       <c r="O4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="24" t="s">
         <v>99</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1323,7 +1451,7 @@
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
-      <c r="I5" s="52"/>
+      <c r="I5" s="36"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
@@ -1333,7 +1461,7 @@
       </c>
       <c r="N5" s="25"/>
       <c r="O5" s="25"/>
-      <c r="Q5" s="54"/>
+      <c r="Q5" s="24"/>
       <c r="R5" s="12" t="s">
         <v>113</v>
       </c>
@@ -1347,22 +1475,22 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
-      <c r="I6" s="52"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="29"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="34"/>
-      <c r="O6" s="35"/>
-      <c r="Q6" s="54"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="29"/>
+      <c r="Q6" s="24"/>
       <c r="R6" s="1" t="s">
         <v>114</v>
       </c>
@@ -1374,7 +1502,7 @@
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="34" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1388,7 +1516,7 @@
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
-      <c r="M7" s="49" t="s">
+      <c r="M7" s="30" t="s">
         <v>34</v>
       </c>
       <c r="N7" s="16" t="s">
@@ -1397,7 +1525,7 @@
       <c r="O7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="54"/>
+      <c r="Q7" s="24"/>
       <c r="R7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1411,50 +1539,50 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="51"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="34" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="49"/>
+      <c r="M8" s="30"/>
       <c r="N8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="54"/>
+      <c r="Q8" s="24"/>
       <c r="R8" s="1" t="s">
         <v>116</v>
       </c>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="E9" s="26" t="s">
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="E9" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="I9" s="52"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="I9" s="36"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="49"/>
+      <c r="M9" s="30"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
         <v>94</v>
@@ -1466,7 +1594,7 @@
       <c r="S9" s="25"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1482,12 +1610,12 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="52"/>
+      <c r="I10" s="36"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="49"/>
+      <c r="M10" s="30"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
         <v>95</v>
@@ -1503,46 +1631,46 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
       <c r="I11" s="25" t="s">
         <v>74</v>
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
-      <c r="M11" s="49"/>
+      <c r="M11" s="30"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q11" s="56" t="s">
+      <c r="Q11" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="56"/>
-      <c r="S11" s="56"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="E12" s="50" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="E12" s="34" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="41" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1563,24 +1691,24 @@
       <c r="S12" s="25"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="51"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="45"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="54" t="s">
+      <c r="M13" s="24" t="s">
         <v>99</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1589,7 +1717,7 @@
       <c r="O13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q13" s="49" t="s">
+      <c r="Q13" s="30" t="s">
         <v>55</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1598,53 +1726,53 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-      <c r="I14" s="22" t="s">
+      <c r="F14" s="39"/>
+      <c r="G14" s="40"/>
+      <c r="I14" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
-      <c r="M14" s="54"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
+      <c r="M14" s="24"/>
       <c r="N14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="Q14" s="49"/>
+      <c r="Q14" s="30"/>
       <c r="R14" s="1" t="s">
         <v>123</v>
       </c>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="E15" s="26" t="s">
+      <c r="B15" s="39"/>
+      <c r="C15" s="40"/>
+      <c r="E15" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
       <c r="I15" s="25" t="s">
         <v>75</v>
       </c>
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
-      <c r="M15" s="22" t="s">
+      <c r="M15" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="23"/>
-      <c r="O15" s="24"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="33"/>
       <c r="Q15" s="25" t="s">
         <v>129</v>
       </c>
@@ -1652,12 +1780,12 @@
       <c r="S15" s="25"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="E16" s="46" t="s">
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="E16" s="50" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1666,17 +1794,17 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="33" t="s">
+      <c r="I16" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="29"/>
       <c r="M16" s="25" t="s">
         <v>105</v>
       </c>
       <c r="N16" s="25"/>
       <c r="O16" s="25"/>
-      <c r="Q16" s="54" t="s">
+      <c r="Q16" s="24" t="s">
         <v>22</v>
       </c>
       <c r="R16" s="1" t="s">
@@ -1687,7 +1815,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="41" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1696,22 +1824,22 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="47"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
-      <c r="M17" s="33" t="s">
+      <c r="J17" s="43"/>
+      <c r="K17" s="29"/>
+      <c r="M17" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="53"/>
-      <c r="O17" s="35"/>
-      <c r="Q17" s="54"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="29"/>
+      <c r="Q17" s="24"/>
       <c r="R17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1720,7 +1848,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1730,7 +1858,7 @@
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="25"/>
-      <c r="I18" s="50" t="s">
+      <c r="I18" s="34" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1739,40 +1867,40 @@
       <c r="K18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="49" t="s">
+      <c r="M18" s="30" t="s">
         <v>34</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="Q18" s="54"/>
+      <c r="Q18" s="24"/>
       <c r="R18" s="1" t="s">
         <v>128</v>
       </c>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="49" t="s">
+      <c r="E19" s="30" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="52"/>
+      <c r="I19" s="36"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="49"/>
+      <c r="M19" s="30"/>
       <c r="N19" s="1" t="s">
         <v>107</v>
       </c>
@@ -1784,22 +1912,22 @@
       <c r="S19" s="25"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="48" t="s">
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="52" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="52"/>
+      <c r="I20" s="36"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="49"/>
+      <c r="M20" s="30"/>
       <c r="N20" s="1" t="s">
         <v>108</v>
       </c>
@@ -1815,7 +1943,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="45" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1824,21 +1952,21 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="49"/>
-      <c r="F21" s="48"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="52"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="51"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M21" s="17"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="55"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
+      <c r="A22" s="45"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1856,16 +1984,16 @@
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="29"/>
       <c r="I23" s="14" t="s">
         <v>85</v>
       </c>
@@ -1875,12 +2003,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
+      <c r="A24" s="45"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="30" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -1899,7 +2027,7 @@
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="49"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -1918,7 +2046,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="49"/>
+      <c r="E26" s="30"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -1936,7 +2064,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="50" t="s">
+      <c r="E28" s="34" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1946,7 +2074,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="51"/>
+      <c r="E29" s="35"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1957,22 +2085,43 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q16:Q18"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q4:Q8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="I3:K3"/>
@@ -1989,43 +2138,22 @@
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q16:Q18"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q4:Q8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q11:S11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2034,19 +2162,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A23382B-C91E-4BC1-BA64-857291C2DF07}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>81</v>
       </c>
@@ -2056,51 +2187,266 @@
       <c r="C1" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="D1" s="60"/>
+      <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="35"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>135</v>
+      </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="63"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="63"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="63"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="63"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="63"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="63"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="63"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="63"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="59"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" s="59"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="59"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="30"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="59"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="59"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="30"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="59"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A8:A21"/>
+    <mergeCell ref="E4:E12"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>

</xml_diff>

<commit_message>
Parts filter added to Bazdid>report 6-2 :triumph:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53C3C36-39D5-49E9-A605-6EB2F2B2FA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F276C6E8-62BC-47B6-BDFA-B1A12EC245A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="174">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -577,6 +577,15 @@
   </si>
   <si>
     <t>داخلی ـ کار روی تکمیل سازی نقشه طرح هما در نرم افزار ویندوزی Map</t>
+  </si>
+  <si>
+    <t>Report 6-2 (Bazdid)</t>
+  </si>
+  <si>
+    <t>frmCumulativeReports.vb</t>
+  </si>
+  <si>
+    <t>spGetReport_6_2 *</t>
   </si>
 </sst>
 </file>
@@ -886,26 +895,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -915,15 +914,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -934,33 +925,54 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -970,35 +982,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1354,58 +1363,58 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40"/>
-      <c r="E2" s="38" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="E2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="I2" s="31" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="I2" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="33"/>
-      <c r="M2" s="31" t="s">
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
+      <c r="M2" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
-      <c r="Q2" s="31" t="s">
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
+      <c r="Q2" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="33"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="31"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="E3" s="55" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="E3" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57"/>
-      <c r="I3" s="25" t="s">
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="I3" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="M3" s="25" t="s">
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="M3" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="Q3" s="25" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="Q3" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1413,12 +1422,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="I4" s="34" t="s">
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
+      <c r="I4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1432,7 +1441,7 @@
       <c r="O4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="61" t="s">
         <v>99</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1441,27 +1450,27 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="E5" s="25" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="E5" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="I5" s="36"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="I5" s="59"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="Q5" s="24"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="Q5" s="61"/>
       <c r="R5" s="12" t="s">
         <v>113</v>
       </c>
@@ -1475,34 +1484,34 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="29"/>
-      <c r="I6" s="36"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42"/>
+      <c r="I6" s="59"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="27" t="s">
+      <c r="M6" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="29"/>
-      <c r="Q6" s="24"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="42"/>
+      <c r="Q6" s="61"/>
       <c r="R6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="E7" s="34" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="E7" s="57" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1511,12 +1520,12 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="M7" s="30" t="s">
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="M7" s="56" t="s">
         <v>34</v>
       </c>
       <c r="N7" s="16" t="s">
@@ -1525,7 +1534,7 @@
       <c r="O7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="24"/>
+      <c r="Q7" s="61"/>
       <c r="R7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1539,62 +1548,62 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="35"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="57" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="30"/>
+      <c r="M8" s="56"/>
       <c r="N8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="24"/>
+      <c r="Q8" s="61"/>
       <c r="R8" s="1" t="s">
         <v>116</v>
       </c>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="E9" s="37" t="s">
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="E9" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="I9" s="36"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="I9" s="59"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="30"/>
+      <c r="M9" s="56"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q9" s="25" t="s">
+      <c r="Q9" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1610,12 +1619,12 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="36"/>
+      <c r="I10" s="59"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="30"/>
+      <c r="M10" s="56"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
         <v>95</v>
@@ -1631,31 +1640,31 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="I11" s="25" t="s">
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="I11" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="M11" s="30"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="M11" s="56"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q11" s="26" t="s">
+      <c r="Q11" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
@@ -1663,14 +1672,14 @@
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="57" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="41" t="s">
+      <c r="I12" s="50" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1679,36 +1688,36 @@
       <c r="K12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="25" t="s">
+      <c r="M12" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="Q12" s="25" t="s">
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="Q12" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="35"/>
+      <c r="E13" s="58"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="42"/>
+      <c r="I13" s="52"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="24" t="s">
+      <c r="M13" s="61" t="s">
         <v>99</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1717,7 +1726,7 @@
       <c r="O13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q13" s="30" t="s">
+      <c r="Q13" s="56" t="s">
         <v>55</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1726,66 +1735,66 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="I14" s="31" t="s">
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="I14" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="32"/>
-      <c r="K14" s="33"/>
-      <c r="M14" s="24"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="31"/>
+      <c r="M14" s="61"/>
       <c r="N14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="Q14" s="30"/>
+      <c r="Q14" s="56"/>
       <c r="R14" s="1" t="s">
         <v>123</v>
       </c>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="E15" s="37" t="s">
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="E15" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="I15" s="25" t="s">
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="I15" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="M15" s="31" t="s">
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="M15" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="32"/>
-      <c r="O15" s="33"/>
-      <c r="Q15" s="25" t="s">
+      <c r="N15" s="30"/>
+      <c r="O15" s="31"/>
+      <c r="Q15" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="E16" s="50" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
+      <c r="E16" s="53" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1794,17 +1803,17 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="43"/>
-      <c r="K16" s="29"/>
-      <c r="M16" s="25" t="s">
+      <c r="J16" s="41"/>
+      <c r="K16" s="42"/>
+      <c r="M16" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="Q16" s="24" t="s">
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="Q16" s="61" t="s">
         <v>22</v>
       </c>
       <c r="R16" s="1" t="s">
@@ -1815,7 +1824,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="50" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1824,22 +1833,22 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="51"/>
+      <c r="E17" s="54"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="43"/>
-      <c r="K17" s="29"/>
-      <c r="M17" s="27" t="s">
+      <c r="J17" s="41"/>
+      <c r="K17" s="42"/>
+      <c r="M17" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="28"/>
-      <c r="O17" s="29"/>
-      <c r="Q17" s="24"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="42"/>
+      <c r="Q17" s="61"/>
       <c r="R17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1848,17 +1857,17 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="I18" s="34" t="s">
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="I18" s="57" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1867,49 +1876,49 @@
       <c r="K18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="30" t="s">
+      <c r="M18" s="56" t="s">
         <v>34</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="Q18" s="24"/>
+      <c r="Q18" s="61"/>
       <c r="R18" s="1" t="s">
         <v>128</v>
       </c>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="56" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="36"/>
+      <c r="I19" s="59"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="30"/>
+      <c r="M19" s="56"/>
       <c r="N19" s="1" t="s">
         <v>107</v>
       </c>
       <c r="O19" s="1"/>
-      <c r="Q19" s="25" t="s">
+      <c r="Q19" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
@@ -1917,17 +1926,17 @@
       </c>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="52" t="s">
+      <c r="E20" s="56"/>
+      <c r="F20" s="55" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="36"/>
+      <c r="I20" s="59"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="30"/>
+      <c r="M20" s="56"/>
       <c r="N20" s="1" t="s">
         <v>108</v>
       </c>
@@ -1943,7 +1952,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="46" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1952,48 +1961,48 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="52"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="55"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="35"/>
+      <c r="I21" s="58"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M21" s="17"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
+      <c r="Q21" s="62"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="62"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="I22" s="25" t="s">
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="I22" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="43"/>
-      <c r="G23" s="29"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="42"/>
       <c r="I23" s="14" t="s">
         <v>85</v>
       </c>
@@ -2003,12 +2012,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="56" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -2017,17 +2026,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="25" t="s">
+      <c r="I24" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="30"/>
+      <c r="E25" s="56"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -2046,7 +2055,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="30"/>
+      <c r="E26" s="56"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -2056,15 +2065,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="57" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -2074,7 +2083,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="35"/>
+      <c r="E29" s="58"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2085,6 +2094,59 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q16:Q18"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q4:Q8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="I24:K24"/>
@@ -2101,59 +2163,6 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q16:Q18"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q4:Q8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q11:S11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2162,10 +2171,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A23382B-C91E-4BC1-BA64-857291C2DF07}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E13" sqref="E13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2196,7 @@
       <c r="C1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="60"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="2" t="s">
         <v>81</v>
       </c>
@@ -2199,42 +2208,42 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="26" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="25" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="30" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="F4" s="65" t="s">
+      <c r="F4" s="28" t="s">
         <v>166</v>
       </c>
       <c r="G4" s="12" t="s">
@@ -2242,15 +2251,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="56" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="30"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="1" t="s">
         <v>168</v>
       </c>
@@ -2259,13 +2268,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="30"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="1" t="s">
         <v>168</v>
       </c>
@@ -2274,13 +2283,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="30"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="1" t="s">
         <v>169</v>
       </c>
@@ -2289,7 +2298,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="56" t="s">
         <v>136</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2298,8 +2307,8 @@
       <c r="C8" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="30"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="1" t="s">
         <v>164</v>
       </c>
@@ -2308,13 +2317,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="30"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="1" t="s">
         <v>165</v>
       </c>
@@ -2323,14 +2332,14 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="65" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="28" t="s">
         <v>167</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -2338,111 +2347,149 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="30"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="56"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D13" s="63"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D14" s="63"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D15" s="63"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="59"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="56"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D17" s="59"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="56"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D18" s="59"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="56"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D19" s="59"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="56"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D20" s="59"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="56"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D21" s="59"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="23"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D22" s="59"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="A8:A21"/>
@@ -2452,6 +2499,8 @@
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Caching before going home :wink:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F276C6E8-62BC-47B6-BDFA-B1A12EC245A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7752EAFD-6E33-47A3-93E7-42383485FE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="187">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -586,6 +586,45 @@
   </si>
   <si>
     <t>spGetReport_6_2 *</t>
+  </si>
+  <si>
+    <t>14th Week (1400/4/19)</t>
+  </si>
+  <si>
+    <t>15th Week (1400/4/26)</t>
+  </si>
+  <si>
+    <t>گلستان ـ بازنویسی گزارش 10-13 با استیمول سافت</t>
+  </si>
+  <si>
+    <t>frmReportSerghatPart.vb</t>
+  </si>
+  <si>
+    <t>Report_10_13.mrt *</t>
+  </si>
+  <si>
+    <t>rptSerghatiPart.rpt</t>
+  </si>
+  <si>
+    <t>داخلی ـ رفع مشکلات مربوط به نقشه طرح هما در نرم افزار ویندوزی</t>
+  </si>
+  <si>
+    <t>frmTraceHistoryData.cs</t>
+  </si>
+  <si>
+    <t>ایلام ـ اضافه شدن فیلتر خط گرم به گزارشات سرویس و اضافه شدن «تجهیزات مصرف شده» به گزارش کلی تجعمی 6-2 ـ ادامه کار</t>
+  </si>
+  <si>
+    <t>امنیت ـ خواندن فایل های گزارش انکد شده در نرم افزار</t>
+  </si>
+  <si>
+    <t>frmReportPreview.vb</t>
+  </si>
+  <si>
+    <t>frmReportPreviewStim.vb</t>
+  </si>
+  <si>
+    <t>Cencryption.cs</t>
   </si>
 </sst>
 </file>
@@ -855,7 +894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -905,6 +944,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -914,7 +973,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -925,6 +992,48 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -932,81 +1041,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1363,58 +1412,58 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="E2" s="34" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="E2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36"/>
-      <c r="I2" s="29" t="s">
+      <c r="F2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="I2" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
-      <c r="M2" s="29" t="s">
+      <c r="J2" s="38"/>
+      <c r="K2" s="39"/>
+      <c r="M2" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
-      <c r="Q2" s="29" t="s">
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
+      <c r="Q2" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="31"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="39"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="E3" s="37" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="E3" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
-      <c r="I3" s="32" t="s">
+      <c r="F3" s="62"/>
+      <c r="G3" s="63"/>
+      <c r="I3" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="M3" s="32" t="s">
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="M3" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="Q3" s="32" t="s">
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="Q3" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1422,12 +1471,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="I4" s="57" t="s">
+      <c r="F4" s="45"/>
+      <c r="G4" s="46"/>
+      <c r="I4" s="40" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1441,7 +1490,7 @@
       <c r="O4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="61" t="s">
+      <c r="Q4" s="30" t="s">
         <v>99</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1450,27 +1499,27 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="E5" s="32" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="E5" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="I5" s="59"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="Q5" s="61"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="Q5" s="30"/>
       <c r="R5" s="12" t="s">
         <v>113</v>
       </c>
@@ -1484,34 +1533,34 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="42"/>
-      <c r="I6" s="59"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="35"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="40" t="s">
+      <c r="M6" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="41"/>
-      <c r="O6" s="42"/>
-      <c r="Q6" s="61"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="35"/>
+      <c r="Q6" s="30"/>
       <c r="R6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="E7" s="57" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="E7" s="40" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1520,12 +1569,12 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="M7" s="56" t="s">
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="M7" s="36" t="s">
         <v>34</v>
       </c>
       <c r="N7" s="16" t="s">
@@ -1534,7 +1583,7 @@
       <c r="O7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="61"/>
+      <c r="Q7" s="30"/>
       <c r="R7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1548,62 +1597,62 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="58"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="40" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="56"/>
+      <c r="M8" s="36"/>
       <c r="N8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="61"/>
+      <c r="Q8" s="30"/>
       <c r="R8" s="1" t="s">
         <v>116</v>
       </c>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="E9" s="33" t="s">
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="E9" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="I9" s="59"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="56"/>
+      <c r="M9" s="36"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q9" s="32" t="s">
+      <c r="Q9" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1619,12 +1668,12 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="59"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="56"/>
+      <c r="M10" s="36"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
         <v>95</v>
@@ -1640,46 +1689,46 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="I11" s="32" t="s">
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="I11" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="M11" s="56"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="M11" s="36"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q11" s="63" t="s">
+      <c r="Q11" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="63"/>
-      <c r="S11" s="63"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="E12" s="57" t="s">
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="E12" s="40" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="50" t="s">
+      <c r="I12" s="47" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1688,36 +1737,36 @@
       <c r="K12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="32" t="s">
+      <c r="M12" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="Q12" s="32" t="s">
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="Q12" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="58"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="52"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="61" t="s">
+      <c r="M13" s="30" t="s">
         <v>99</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1726,7 +1775,7 @@
       <c r="O13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q13" s="56" t="s">
+      <c r="Q13" s="36" t="s">
         <v>55</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1735,66 +1784,66 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
-      <c r="I14" s="29" t="s">
+      <c r="F14" s="45"/>
+      <c r="G14" s="46"/>
+      <c r="I14" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="31"/>
-      <c r="M14" s="61"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+      <c r="M14" s="30"/>
       <c r="N14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="Q14" s="56"/>
+      <c r="Q14" s="36"/>
       <c r="R14" s="1" t="s">
         <v>123</v>
       </c>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="E15" s="33" t="s">
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
+      <c r="E15" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="I15" s="32" t="s">
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="I15" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="M15" s="29" t="s">
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="M15" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="30"/>
-      <c r="O15" s="31"/>
-      <c r="Q15" s="32" t="s">
+      <c r="N15" s="38"/>
+      <c r="O15" s="39"/>
+      <c r="Q15" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
-      <c r="E16" s="53" t="s">
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="E16" s="56" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1803,17 +1852,17 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="40" t="s">
+      <c r="I16" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="41"/>
-      <c r="K16" s="42"/>
-      <c r="M16" s="32" t="s">
+      <c r="J16" s="49"/>
+      <c r="K16" s="35"/>
+      <c r="M16" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="Q16" s="61" t="s">
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="Q16" s="30" t="s">
         <v>22</v>
       </c>
       <c r="R16" s="1" t="s">
@@ -1824,7 +1873,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="47" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1833,22 +1882,22 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="54"/>
+      <c r="E17" s="57"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="I17" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="41"/>
-      <c r="K17" s="42"/>
-      <c r="M17" s="40" t="s">
+      <c r="J17" s="49"/>
+      <c r="K17" s="35"/>
+      <c r="M17" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="60"/>
-      <c r="O17" s="42"/>
-      <c r="Q17" s="61"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="35"/>
+      <c r="Q17" s="30"/>
       <c r="R17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1857,17 +1906,17 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="I18" s="57" t="s">
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="I18" s="40" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1876,67 +1925,67 @@
       <c r="K18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="56" t="s">
+      <c r="M18" s="36" t="s">
         <v>34</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="Q18" s="61"/>
+      <c r="Q18" s="30"/>
       <c r="R18" s="1" t="s">
         <v>128</v>
       </c>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="56" t="s">
+      <c r="E19" s="36" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="59"/>
+      <c r="I19" s="42"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="56"/>
+      <c r="M19" s="36"/>
       <c r="N19" s="1" t="s">
         <v>107</v>
       </c>
       <c r="O19" s="1"/>
-      <c r="Q19" s="32" t="s">
+      <c r="Q19" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="R19" s="32"/>
-      <c r="S19" s="32"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="55" t="s">
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="58" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="59"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="56"/>
+      <c r="M20" s="36"/>
       <c r="N20" s="1" t="s">
         <v>108</v>
       </c>
@@ -1952,7 +2001,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="51" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1961,48 +2010,48 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="56"/>
-      <c r="F21" s="55"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="58"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="58"/>
+      <c r="I21" s="41"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M21" s="17"/>
-      <c r="Q21" s="62"/>
-      <c r="R21" s="62"/>
-      <c r="S21" s="62"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="I22" s="32" t="s">
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="I22" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="42"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="35"/>
       <c r="I23" s="14" t="s">
         <v>85</v>
       </c>
@@ -2012,12 +2061,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="56" t="s">
+      <c r="E24" s="36" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -2026,17 +2075,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="32" t="s">
+      <c r="I24" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="56"/>
+      <c r="E25" s="36"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -2055,7 +2104,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="56"/>
+      <c r="E26" s="36"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -2065,15 +2114,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="57" t="s">
+      <c r="E28" s="40" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -2083,7 +2132,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="58"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2094,22 +2143,43 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q16:Q18"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q4:Q8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E23:G23"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="I3:K3"/>
@@ -2126,43 +2196,22 @@
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q16:Q18"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q4:Q8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q11:S11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2171,10 +2220,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A23382B-C91E-4BC1-BA64-857291C2DF07}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:G13"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,17 +2257,17 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
@@ -2228,7 +2277,7 @@
       <c r="C3" s="64"/>
       <c r="D3" s="26"/>
       <c r="E3" s="32" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
@@ -2240,18 +2289,14 @@
       <c r="B4" s="65"/>
       <c r="C4" s="65"/>
       <c r="D4" s="24"/>
-      <c r="E4" s="56" t="s">
-        <v>153</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>154</v>
-      </c>
+      <c r="E4" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2259,46 +2304,48 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="27"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>156</v>
+      <c r="E5" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="27"/>
-      <c r="E6" s="56"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="1" t="s">
         <v>168</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="36" t="s">
         <v>136</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2308,199 +2355,275 @@
         <v>155</v>
       </c>
       <c r="D8" s="27"/>
-      <c r="E8" s="56"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D9" s="27"/>
-      <c r="E9" s="56"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D10" s="27"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="28" t="s">
-        <v>167</v>
+      <c r="E10" s="36"/>
+      <c r="F10" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>140</v>
       </c>
       <c r="D11" s="27"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="1"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="28" t="s">
+        <v>167</v>
+      </c>
       <c r="G11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>141</v>
       </c>
       <c r="D12" s="27"/>
-      <c r="E12" s="56"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D13" s="27"/>
-      <c r="E13" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D14" s="27"/>
-      <c r="E14" s="50" t="s">
-        <v>136</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>171</v>
-      </c>
+      <c r="E14" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D15" s="27"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>173</v>
-      </c>
+      <c r="E15" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D16" s="23"/>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
+      <c r="E16" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D17" s="23"/>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D18" s="23"/>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>148</v>
       </c>
       <c r="D19" s="23"/>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
+      <c r="E19" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>149</v>
       </c>
       <c r="D20" s="23"/>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
+      <c r="E20" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>150</v>
       </c>
       <c r="D21" s="23"/>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="36"/>
+      <c r="F21" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D22" s="23"/>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="17"/>
+      <c r="E22" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="36"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="69" t="s">
+        <v>183</v>
+      </c>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="36"/>
+      <c r="F27" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="36"/>
+      <c r="F28" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G28" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="19">
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A8:A21"/>
-    <mergeCell ref="E4:E12"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:E13"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A8:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data Gathering Done :wink:
</commit_message>
<xml_diff>
--- a/Data/Data Gathering.xlsx
+++ b/Data/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96471D1C-F03A-4E3D-B8D3-2AC314965F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB81D78-94FD-43B8-8A9A-81A1448D5239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="239">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -695,12 +695,99 @@
   <si>
     <t>ایلام ـ ارسال پیامک حاوی کد اجازه کار به اکیپ عملیاتی</t>
   </si>
+  <si>
+    <t>ایلام ـ نمایش ستون تاریخ و ساعت عودت درخواست در مانیتورینگ درخواست خاموشی بابرنامه</t>
+  </si>
+  <si>
+    <t>ViewTamirRequest </t>
+  </si>
+  <si>
+    <t>17th Week (1400/5/09)</t>
+  </si>
+  <si>
+    <t>داخلی ـ تغییرات در بخش نمایش خاموشی‌ها روی نقشه در مانیتورینگ حوادث</t>
+  </si>
+  <si>
+    <t>frmHomaEndOnCall.vb</t>
+  </si>
+  <si>
+    <t>frmHomaOnCallHistory.vb</t>
+  </si>
+  <si>
+    <t>TazarvMapUC_Cars.cs</t>
+  </si>
+  <si>
+    <t>frmCars.cs</t>
+  </si>
+  <si>
+    <t>frmCarsData.cs</t>
+  </si>
+  <si>
+    <t>frmMonitoringTamirRewquest.vb</t>
+  </si>
+  <si>
+    <t>18th Week (1400/5/16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">یزد ـ کشف آسیب پذیری اعلام شده با موضوع Cross Site Scripting در نسخه گزارشگیر نرم افزار تحت وب </t>
+  </si>
+  <si>
+    <t>TZHavades_2013</t>
+  </si>
+  <si>
+    <t>Globaz.asax.cs</t>
+  </si>
+  <si>
+    <t>Oops.asax.cs</t>
+  </si>
+  <si>
+    <t>Web.config</t>
+  </si>
+  <si>
+    <t>بوشهر ـ اضافه نمودن کد پست توزیع به مانیتورینگ هما و بخش تکمیل پرونده مطابق نامه پیوست</t>
+  </si>
+  <si>
+    <t>&lt;Config-Script&gt;</t>
+  </si>
+  <si>
+    <t>frmNewRequestsPreview.vb</t>
+  </si>
+  <si>
+    <t>لرستان ـ ایجاد دو گزارش جدید زیر در نرم افزار ثبت حوادث</t>
+  </si>
+  <si>
+    <t>Report_14_5.mrt</t>
+  </si>
+  <si>
+    <t>frmHomaReportRequest.vb</t>
+  </si>
+  <si>
+    <t>Havades_App.vbproj</t>
+  </si>
+  <si>
+    <t>HomaReportArea(2-h).mrt</t>
+  </si>
+  <si>
+    <t>spHomaReportArea</t>
+  </si>
+  <si>
+    <t>HomaStatisticsReport</t>
+  </si>
+  <si>
+    <t>شمال کرمان ـ اجرای بند 2 نامه پیوست (ادامه)</t>
+  </si>
+  <si>
+    <t>Bargh_Reports</t>
+  </si>
+  <si>
+    <t>frmReportUtilizationFactor.vb</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,6 +851,19 @@
     <font>
       <sz val="10.7"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -969,7 +1069,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1023,6 +1123,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1122,27 +1230,21 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1431,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" view="pageBreakPreview" topLeftCell="J1" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView rightToLeft="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="M7" sqref="M7:M11"/>
     </sheetView>
   </sheetViews>
@@ -1499,58 +1601,58 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="E2" s="36" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="E2" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="I2" s="31" t="s">
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="I2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="33"/>
-      <c r="M2" s="31" t="s">
+      <c r="J2" s="36"/>
+      <c r="K2" s="37"/>
+      <c r="M2" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
-      <c r="Q2" s="31" t="s">
+      <c r="N2" s="36"/>
+      <c r="O2" s="37"/>
+      <c r="Q2" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="33"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="37"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="E3" s="39" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="E3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="I3" s="34" t="s">
+      <c r="F3" s="44"/>
+      <c r="G3" s="45"/>
+      <c r="I3" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="M3" s="34" t="s">
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="M3" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="Q3" s="34" t="s">
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="Q3" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1558,12 +1660,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
-      <c r="I4" s="59" t="s">
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
+      <c r="I4" s="63" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1577,7 +1679,7 @@
       <c r="O4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="63" t="s">
+      <c r="Q4" s="67" t="s">
         <v>99</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1586,27 +1688,27 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="E5" s="34" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="E5" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="I5" s="61"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="I5" s="65"/>
       <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="34" t="s">
+      <c r="M5" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="Q5" s="63"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="Q5" s="67"/>
       <c r="R5" s="12" t="s">
         <v>113</v>
       </c>
@@ -1620,34 +1722,34 @@
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
-      <c r="I6" s="61"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="48"/>
+      <c r="I6" s="65"/>
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="42" t="s">
+      <c r="M6" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="44"/>
-      <c r="Q6" s="63"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="48"/>
+      <c r="Q6" s="67"/>
       <c r="R6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="E7" s="59" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="E7" s="63" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1656,12 +1758,12 @@
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="M7" s="58" t="s">
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="M7" s="62" t="s">
         <v>34</v>
       </c>
       <c r="N7" s="16" t="s">
@@ -1670,7 +1772,7 @@
       <c r="O7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="63"/>
+      <c r="Q7" s="67"/>
       <c r="R7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1684,62 +1786,62 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="60"/>
+      <c r="E8" s="64"/>
       <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="63" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="58"/>
+      <c r="M8" s="62"/>
       <c r="N8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="63"/>
+      <c r="Q8" s="67"/>
       <c r="R8" s="1" t="s">
         <v>116</v>
       </c>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="E9" s="35" t="s">
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="E9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="I9" s="61"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="I9" s="65"/>
       <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="58"/>
+      <c r="M9" s="62"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="Q9" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1755,12 +1857,12 @@
       <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="61"/>
+      <c r="I10" s="65"/>
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="58"/>
+      <c r="M10" s="62"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
         <v>95</v>
@@ -1776,46 +1878,46 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="I11" s="34" t="s">
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="I11" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="M11" s="58"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="M11" s="62"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q11" s="65" t="s">
+      <c r="Q11" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
+      <c r="R11" s="69"/>
+      <c r="S11" s="69"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="E12" s="59" t="s">
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="E12" s="63" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="52" t="s">
+      <c r="I12" s="56" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1824,36 +1926,36 @@
       <c r="K12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="34" t="s">
+      <c r="M12" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="Q12" s="34" t="s">
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="Q12" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="60"/>
+      <c r="E13" s="64"/>
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="I13" s="54"/>
+      <c r="I13" s="58"/>
       <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="63" t="s">
+      <c r="M13" s="67" t="s">
         <v>99</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1862,7 +1964,7 @@
       <c r="O13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q13" s="58" t="s">
+      <c r="Q13" s="62" t="s">
         <v>55</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1871,66 +1973,66 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
-      <c r="I14" s="31" t="s">
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
+      <c r="I14" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="32"/>
-      <c r="K14" s="33"/>
-      <c r="M14" s="63"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="37"/>
+      <c r="M14" s="67"/>
       <c r="N14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="Q14" s="58"/>
+      <c r="Q14" s="62"/>
       <c r="R14" s="1" t="s">
         <v>123</v>
       </c>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="E15" s="35" t="s">
+      <c r="B15" s="41"/>
+      <c r="C15" s="42"/>
+      <c r="E15" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="I15" s="34" t="s">
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="I15" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="M15" s="31" t="s">
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="M15" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="32"/>
-      <c r="O15" s="33"/>
-      <c r="Q15" s="34" t="s">
+      <c r="N15" s="36"/>
+      <c r="O15" s="37"/>
+      <c r="Q15" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
-      <c r="E16" s="55" t="s">
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+      <c r="E16" s="59" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1939,17 +2041,17 @@
       <c r="G16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="42" t="s">
+      <c r="I16" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="43"/>
-      <c r="K16" s="44"/>
-      <c r="M16" s="34" t="s">
+      <c r="J16" s="47"/>
+      <c r="K16" s="48"/>
+      <c r="M16" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="Q16" s="63" t="s">
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="Q16" s="67" t="s">
         <v>22</v>
       </c>
       <c r="R16" s="1" t="s">
@@ -1960,7 +2062,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="56" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1969,22 +2071,22 @@
       <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="56"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="42" t="s">
+      <c r="I17" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="43"/>
-      <c r="K17" s="44"/>
-      <c r="M17" s="42" t="s">
+      <c r="J17" s="47"/>
+      <c r="K17" s="48"/>
+      <c r="M17" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="62"/>
-      <c r="O17" s="44"/>
-      <c r="Q17" s="63"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="48"/>
+      <c r="Q17" s="67"/>
       <c r="R17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1993,17 +2095,17 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="I18" s="59" t="s">
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="I18" s="63" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -2012,67 +2114,67 @@
       <c r="K18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="58" t="s">
+      <c r="M18" s="62" t="s">
         <v>34</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="Q18" s="63"/>
+      <c r="Q18" s="67"/>
       <c r="R18" s="1" t="s">
         <v>128</v>
       </c>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="58" t="s">
+      <c r="E19" s="62" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="61"/>
+      <c r="I19" s="65"/>
       <c r="J19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="58"/>
+      <c r="M19" s="62"/>
       <c r="N19" s="1" t="s">
         <v>107</v>
       </c>
       <c r="O19" s="1"/>
-      <c r="Q19" s="34" t="s">
+      <c r="Q19" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="R19" s="34"/>
-      <c r="S19" s="34"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="57" t="s">
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="61" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="61"/>
+      <c r="I20" s="65"/>
       <c r="J20" s="1"/>
       <c r="K20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="58"/>
+      <c r="M20" s="62"/>
       <c r="N20" s="1" t="s">
         <v>108</v>
       </c>
@@ -2088,7 +2190,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="52" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2097,48 +2199,48 @@
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="58"/>
-      <c r="F21" s="57"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="61"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="60"/>
+      <c r="I21" s="64"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M21" s="17"/>
-      <c r="Q21" s="64"/>
-      <c r="R21" s="64"/>
-      <c r="S21" s="64"/>
+      <c r="Q21" s="68"/>
+      <c r="R21" s="68"/>
+      <c r="S21" s="68"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
+      <c r="A22" s="52"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="I22" s="34" t="s">
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="I22" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
+      <c r="A23" s="52"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
       <c r="I23" s="14" t="s">
         <v>85</v>
       </c>
@@ -2148,12 +2250,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="62" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -2162,17 +2264,17 @@
       <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="58"/>
+      <c r="E25" s="62"/>
       <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
@@ -2191,7 +2293,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="58"/>
+      <c r="E26" s="62"/>
       <c r="F26" s="11"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
@@ -2201,15 +2303,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="E28" s="59" t="s">
+      <c r="E28" s="63" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -2219,7 +2321,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="E29" s="60"/>
+      <c r="E29" s="64"/>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2307,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A23382B-C91E-4BC1-BA64-857291C2DF07}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20:K20"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,9 +2423,10 @@
     <col min="6" max="6" width="32.85546875" customWidth="1"/>
     <col min="7" max="7" width="30.7109375" customWidth="1"/>
     <col min="9" max="11" width="30.7109375" customWidth="1"/>
+    <col min="13" max="15" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>81</v>
       </c>
@@ -2352,63 +2455,89 @@
       <c r="K1" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="M1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="69" t="s">
         <v>152</v>
       </c>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="I2" s="65" t="s">
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="I2" s="69" t="s">
         <v>187</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="M2" s="69" t="s">
+        <v>220</v>
+      </c>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
       <c r="D3" s="26"/>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="69" t="s">
         <v>174</v>
       </c>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="I3" s="34" t="s">
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="I3" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="M3" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="24"/>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="I4" s="34" t="s">
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="I4" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="M4" s="67" t="s">
+        <v>222</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="62" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2416,7 +2545,7 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="27"/>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="62" t="s">
         <v>153</v>
       </c>
       <c r="F5" s="28" t="s">
@@ -2425,54 +2554,69 @@
       <c r="G5" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="44"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="48"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="62"/>
       <c r="B6" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="27"/>
-      <c r="E6" s="58"/>
+      <c r="E6" s="62"/>
       <c r="F6" s="1" t="s">
         <v>168</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="58"/>
+      <c r="E7" s="62"/>
       <c r="F7" s="1" t="s">
         <v>168</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="J7" s="43"/>
-      <c r="K7" s="44"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
+      <c r="M7" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="62" t="s">
         <v>136</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2482,34 +2626,43 @@
         <v>155</v>
       </c>
       <c r="D8" s="27"/>
-      <c r="E8" s="58"/>
+      <c r="E8" s="62"/>
       <c r="F8" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="46" t="s">
         <v>193</v>
       </c>
-      <c r="J8" s="43"/>
-      <c r="K8" s="44"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="M8" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D9" s="27"/>
-      <c r="E9" s="58"/>
+      <c r="E9" s="62"/>
       <c r="F9" s="1" t="s">
         <v>164</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I9" s="58" t="s">
+      <c r="I9" s="62" t="s">
         <v>34</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -2518,255 +2671,308 @@
       <c r="K9" s="12" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
+      <c r="M9" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="62"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D10" s="27"/>
-      <c r="E10" s="58"/>
+      <c r="E10" s="62"/>
       <c r="F10" s="1" t="s">
         <v>165</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I10" s="58"/>
+      <c r="I10" s="62"/>
       <c r="J10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
+      <c r="M10" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="62"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>140</v>
       </c>
       <c r="D11" s="27"/>
-      <c r="E11" s="58"/>
+      <c r="E11" s="62"/>
       <c r="F11" s="28" t="s">
         <v>167</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I11" s="58"/>
+      <c r="I11" s="62"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="62"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>141</v>
       </c>
       <c r="D12" s="27"/>
-      <c r="E12" s="58"/>
+      <c r="E12" s="62"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I12" s="58"/>
+      <c r="I12" s="62"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="62"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D13" s="27"/>
-      <c r="E13" s="58"/>
+      <c r="E13" s="62"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I13" s="58"/>
+      <c r="I13" s="62"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
+      <c r="M13" s="71"/>
+      <c r="N13" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="62"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D14" s="27"/>
-      <c r="E14" s="65" t="s">
+      <c r="E14" s="69" t="s">
         <v>175</v>
       </c>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="I14" s="34" t="s">
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="I14" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="62"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D15" s="27"/>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="I15" s="58" t="s">
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="I15" s="62" t="s">
         <v>201</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>202</v>
       </c>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
+      <c r="M15" s="71"/>
+      <c r="N15" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="62"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D16" s="23"/>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="70" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>177</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="I16" s="58"/>
+      <c r="I16" s="62"/>
       <c r="J16" s="1" t="s">
         <v>203</v>
       </c>
       <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
+      <c r="M16" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="62"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D17" s="23"/>
-      <c r="E17" s="68"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="1" t="s">
         <v>178</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="I17" s="58"/>
+      <c r="I17" s="62"/>
       <c r="J17" s="1" t="s">
         <v>204</v>
       </c>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
+      <c r="M17" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="62"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D18" s="23"/>
-      <c r="E18" s="68"/>
+      <c r="E18" s="71"/>
       <c r="F18" s="30" t="s">
         <v>179</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="I18" s="58"/>
+      <c r="I18" s="62"/>
       <c r="J18" s="1" t="s">
         <v>205</v>
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="62"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>148</v>
       </c>
       <c r="D19" s="23"/>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="I19" s="58"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="I19" s="62"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="62"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>149</v>
       </c>
       <c r="D20" s="23"/>
-      <c r="E20" s="58" t="s">
+      <c r="E20" s="62" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>168</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="62"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>150</v>
       </c>
       <c r="D21" s="23"/>
-      <c r="E21" s="58"/>
+      <c r="E21" s="62"/>
       <c r="F21" s="1" t="s">
         <v>181</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="I21" s="71" t="s">
+      <c r="I21" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="J21" s="72" t="s">
+      <c r="J21" s="75" t="s">
         <v>207</v>
       </c>
-      <c r="K21" s="72"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
+      <c r="K21" s="75"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="62"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D22" s="23"/>
-      <c r="E22" s="66" t="s">
+      <c r="E22" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="I22" s="34" t="s">
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="I22" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="58" t="s">
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E23" s="62" t="s">
         <v>136</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -2783,46 +2989,111 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="58"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E24" s="62"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I24" s="73"/>
-    </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="66" t="s">
+      <c r="I24" s="69" t="s">
+        <v>212</v>
+      </c>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+    </row>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="58" t="s">
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="I25" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E26" s="62" t="s">
         <v>22</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>184</v>
       </c>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="58"/>
+      <c r="I26" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="K26" s="33" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E27" s="62"/>
       <c r="F27" s="1" t="s">
         <v>185</v>
       </c>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E28" s="58"/>
+      <c r="I27" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E28" s="62"/>
       <c r="F28" s="1" t="s">
         <v>186</v>
       </c>
       <c r="G28" s="1"/>
+      <c r="I28" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I29" s="62"/>
+      <c r="J29" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I30" s="62"/>
+      <c r="J30" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I31" s="62"/>
+      <c r="J31" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I32" s="62"/>
+      <c r="J32" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I33" s="62"/>
+      <c r="J33" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K33" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="43">
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="A8:A22"/>
@@ -2855,6 +3126,17 @@
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E23:E24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:I33"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:M15"/>
+    <mergeCell ref="M16:O16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>